<commit_message>
Map Icons placed normally, and N/A layers now present.
</commit_message>
<xml_diff>
--- a/src/context/Dangermond_LithologicLogs.xlsx
+++ b/src/context/Dangermond_LithologicLogs.xlsx
@@ -285,7 +285,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +296,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -332,16 +338,16 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2634,7 +2640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -2704,7 +2710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -2739,7 +2745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
@@ -2774,7 +2780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
         <v>71</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
         <v>74</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -3124,7 +3130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
@@ -3159,7 +3165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -3194,7 +3200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -3264,7 +3270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -3334,7 +3340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -3369,7 +3375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="1" t="s">
         <v>82</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
@@ -3509,7 +3515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
@@ -3544,7 +3550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -3579,7 +3585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>

</xml_diff>